<commit_message>
Cambios hasta el 30 de noviembre de 2022
</commit_message>
<xml_diff>
--- a/base de datos/covid_zmvm shp/Diccionario.xlsx
+++ b/base de datos/covid_zmvm shp/Diccionario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jprud\Desktop\EE-Practicas\Práctica 2\covid_zmvm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Analisis-de-datos-espaciales\base de datos\covid_zmvm shp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DD9160-B1DC-4521-B209-919BD0D0E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5648C0-FC6B-4B21-BE76-94E604573FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{630CFB02-0148-4456-B6D2-E22D83A3071D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{630CFB02-0148-4456-B6D2-E22D83A3071D}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>poind</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>Versiones logarítmicas</t>
+  </si>
+  <si>
+    <t>idh2015</t>
+  </si>
+  <si>
+    <t>Índice de desarrollo humano, 2015</t>
   </si>
 </sst>
 </file>
@@ -784,9 +790,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE75008-545D-467B-95F6-2DA68B0970EB}">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1166,132 +1174,131 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="68" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
     </row>
     <row r="69" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G69" s="1"/>
@@ -1392,14 +1399,14 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="81" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
+    <row r="80" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
     </row>
     <row r="82" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G82" s="1"/>
@@ -1446,6 +1453,15 @@
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
     </row>
+    <row r="87" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>